<commit_message>
Updates for 7 May
</commit_message>
<xml_diff>
--- a/data/us/mac_us_states_deaths.xlsx
+++ b/data/us/mac_us_states_deaths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/71ffaa969b2b2dbb/Meridian/h Computer Science/Teacher Projects/COVID/data/us/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="114_{53F5A8DB-8100-4239-9BB5-93B3786D6557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{81035F52-62BB-4CE6-AC4A-A3CF00FBA7D0}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="114_{53F5A8DB-8100-4239-9BB5-93B3786D6557}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1D6431FC-E143-402C-A63B-9F725DD6D96E}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="710" windowWidth="22490" windowHeight="16670" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
+    <workbookView xWindow="2470" yWindow="1120" windowWidth="22490" windowHeight="16480" xr2:uid="{479F01FD-FBEA-480D-8311-3224064F669A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>New York</t>
   </si>
@@ -357,6 +357,9 @@
   </si>
   <si>
     <t xml:space="preserve"> 5/5/20</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5/6/20</t>
   </si>
 </sst>
 </file>
@@ -817,10 +820,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07C58A35-5762-462F-A8C8-AA6852158F40}">
-  <dimension ref="A1:BB56"/>
+  <dimension ref="A1:BC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -830,7 +833,7 @@
     <col min="21" max="21" width="8.7265625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>44</v>
       </c>
@@ -993,8 +996,11 @@
       <c r="BB1" s="3" t="s">
         <v>106</v>
       </c>
+      <c r="BC1" s="3" t="s">
+        <v>107</v>
+      </c>
     </row>
-    <row r="2" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1157,8 +1163,11 @@
       <c r="BB2" s="10">
         <v>315</v>
       </c>
+      <c r="BC2" s="10">
+        <v>343</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
@@ -1321,8 +1330,11 @@
       <c r="BB3" s="10">
         <v>9</v>
       </c>
+      <c r="BC3" s="10">
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1485,8 +1497,11 @@
       <c r="BB4" s="10">
         <v>395</v>
       </c>
+      <c r="BC4" s="10">
+        <v>426</v>
+      </c>
     </row>
-    <row r="5" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
         <v>28</v>
       </c>
@@ -1649,8 +1664,11 @@
       <c r="BB5" s="10">
         <v>83</v>
       </c>
+      <c r="BC5" s="10">
+        <v>87</v>
+      </c>
     </row>
-    <row r="6" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1813,8 +1831,11 @@
       <c r="BB6" s="10">
         <v>2379</v>
       </c>
+      <c r="BC6" s="10">
+        <v>2462</v>
+      </c>
     </row>
-    <row r="7" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1977,8 +1998,11 @@
       <c r="BB7" s="10">
         <v>903</v>
       </c>
+      <c r="BC7" s="10">
+        <v>921</v>
+      </c>
     </row>
-    <row r="8" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -2141,8 +2165,11 @@
       <c r="BB8" s="10">
         <v>2633</v>
       </c>
+      <c r="BC8" s="10">
+        <v>2718</v>
+      </c>
     </row>
-    <row r="9" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
@@ -2305,8 +2332,11 @@
       <c r="BB9" s="10">
         <v>187</v>
       </c>
+      <c r="BC9" s="10">
+        <v>193</v>
+      </c>
     </row>
-    <row r="10" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -2469,8 +2499,11 @@
       <c r="BB10" s="10">
         <v>264</v>
       </c>
+      <c r="BC10" s="10">
+        <v>277</v>
+      </c>
     </row>
-    <row r="11" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
@@ -2633,8 +2666,11 @@
       <c r="BB11" s="10">
         <v>1471</v>
       </c>
+      <c r="BC11" s="10">
+        <v>1539</v>
+      </c>
     </row>
-    <row r="12" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
@@ -2797,8 +2833,11 @@
       <c r="BB12" s="10">
         <v>1295</v>
       </c>
+      <c r="BC12" s="10">
+        <v>1327</v>
+      </c>
     </row>
-    <row r="13" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -2961,8 +3000,11 @@
       <c r="BB13" s="10">
         <v>5</v>
       </c>
+      <c r="BC13" s="10">
+        <v>5</v>
+      </c>
     </row>
-    <row r="14" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
         <v>61</v>
       </c>
@@ -3125,8 +3167,11 @@
       <c r="BB14" s="10">
         <v>17</v>
       </c>
+      <c r="BC14" s="10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="15" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
         <v>32</v>
       </c>
@@ -3289,8 +3334,11 @@
       <c r="BB15" s="10">
         <v>65</v>
       </c>
+      <c r="BC15" s="10">
+        <v>66</v>
+      </c>
     </row>
-    <row r="16" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -3453,8 +3501,11 @@
       <c r="BB16" s="10">
         <v>2838</v>
       </c>
+      <c r="BC16" s="10">
+        <v>2974</v>
+      </c>
     </row>
-    <row r="17" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -3617,8 +3668,11 @@
       <c r="BB17" s="10">
         <v>1326</v>
       </c>
+      <c r="BC17" s="10">
+        <v>1377</v>
+      </c>
     </row>
-    <row r="18" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
         <v>38</v>
       </c>
@@ -3781,8 +3835,11 @@
       <c r="BB18" s="10">
         <v>207</v>
       </c>
+      <c r="BC18" s="10">
+        <v>219</v>
+      </c>
     </row>
-    <row r="19" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -3945,8 +4002,11 @@
       <c r="BB19" s="10">
         <v>161</v>
       </c>
+      <c r="BC19" s="10">
+        <v>164</v>
+      </c>
     </row>
-    <row r="20" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -4109,8 +4169,11 @@
       <c r="BB20" s="10">
         <v>275</v>
       </c>
+      <c r="BC20" s="10">
+        <v>283</v>
+      </c>
     </row>
-    <row r="21" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -4273,8 +4336,11 @@
       <c r="BB21" s="10">
         <v>2115</v>
       </c>
+      <c r="BC21" s="10">
+        <v>2167</v>
+      </c>
     </row>
-    <row r="22" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="1" t="s">
         <v>63</v>
       </c>
@@ -4437,8 +4503,11 @@
       <c r="BB22" s="10">
         <v>61</v>
       </c>
+      <c r="BC22" s="10">
+        <v>62</v>
+      </c>
     </row>
-    <row r="23" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="1" t="s">
         <v>27</v>
       </c>
@@ -4601,8 +4670,11 @@
       <c r="BB23" s="10">
         <v>1390</v>
       </c>
+      <c r="BC23" s="10">
+        <v>1437</v>
+      </c>
     </row>
-    <row r="24" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -4765,8 +4837,11 @@
       <c r="BB24" s="10">
         <v>4212</v>
       </c>
+      <c r="BC24" s="10">
+        <v>4420</v>
+      </c>
     </row>
-    <row r="25" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -4929,8 +5004,11 @@
       <c r="BB25" s="10">
         <v>4179</v>
       </c>
+      <c r="BC25" s="10">
+        <v>4250</v>
+      </c>
     </row>
-    <row r="26" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -5093,8 +5171,11 @@
       <c r="BB26" s="10">
         <v>455</v>
       </c>
+      <c r="BC26" s="10">
+        <v>485</v>
+      </c>
     </row>
-    <row r="27" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -5257,8 +5338,11 @@
       <c r="BB27" s="10">
         <v>342</v>
       </c>
+      <c r="BC27" s="10">
+        <v>374</v>
+      </c>
     </row>
-    <row r="28" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -5421,8 +5505,11 @@
       <c r="BB28" s="10">
         <v>409</v>
       </c>
+      <c r="BC28" s="10">
+        <v>425</v>
+      </c>
     </row>
-    <row r="29" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
@@ -5585,8 +5672,11 @@
       <c r="BB29" s="10">
         <v>16</v>
       </c>
+      <c r="BC29" s="10">
+        <v>16</v>
+      </c>
     </row>
-    <row r="30" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="1" t="s">
         <v>59</v>
       </c>
@@ -5749,8 +5839,11 @@
       <c r="BB30" s="10">
         <v>82</v>
       </c>
+      <c r="BC30" s="10">
+        <v>86</v>
+      </c>
     </row>
-    <row r="31" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -5913,8 +6006,11 @@
       <c r="BB31" s="10">
         <v>276</v>
       </c>
+      <c r="BC31" s="10">
+        <v>286</v>
+      </c>
     </row>
-    <row r="32" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="1" t="s">
         <v>39</v>
       </c>
@@ -6077,8 +6173,11 @@
       <c r="BB32" s="10">
         <v>92</v>
       </c>
+      <c r="BC32" s="10">
+        <v>111</v>
+      </c>
     </row>
-    <row r="33" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -6241,8 +6340,11 @@
       <c r="BB33" s="10">
         <v>8292</v>
       </c>
+      <c r="BC33" s="10">
+        <v>8572</v>
+      </c>
     </row>
-    <row r="34" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -6405,8 +6507,11 @@
       <c r="BB34" s="10">
         <v>162</v>
       </c>
+      <c r="BC34" s="10">
+        <v>169</v>
+      </c>
     </row>
-    <row r="35" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="1" t="s">
         <v>0</v>
       </c>
@@ -6569,8 +6674,11 @@
       <c r="BB35" s="10">
         <v>25204</v>
       </c>
+      <c r="BC35" s="10">
+        <v>25956</v>
+      </c>
     </row>
-    <row r="36" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -6733,8 +6841,11 @@
       <c r="BB36" s="10">
         <v>470</v>
       </c>
+      <c r="BC36" s="10">
+        <v>493</v>
+      </c>
     </row>
-    <row r="37" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="1" t="s">
         <v>65</v>
       </c>
@@ -6897,8 +7008,11 @@
       <c r="BB37" s="10">
         <v>25</v>
       </c>
+      <c r="BC37" s="10">
+        <v>31</v>
+      </c>
     </row>
-    <row r="38" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="1" t="s">
         <v>15</v>
       </c>
@@ -7061,8 +7175,11 @@
       <c r="BB38" s="10">
         <v>1136</v>
       </c>
+      <c r="BC38" s="10">
+        <v>1225</v>
+      </c>
     </row>
-    <row r="39" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="1" t="s">
         <v>24</v>
       </c>
@@ -7225,8 +7342,11 @@
       <c r="BB39" s="10">
         <v>247</v>
       </c>
+      <c r="BC39" s="10">
+        <v>253</v>
+      </c>
     </row>
-    <row r="40" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="1" t="s">
         <v>17</v>
       </c>
@@ -7389,8 +7509,11 @@
       <c r="BB40" s="10">
         <v>113</v>
       </c>
+      <c r="BC40" s="10">
+        <v>115</v>
+      </c>
     </row>
-    <row r="41" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="1" t="s">
         <v>14</v>
       </c>
@@ -7553,8 +7676,11 @@
       <c r="BB41" s="10">
         <v>3196</v>
       </c>
+      <c r="BC41" s="10">
+        <v>3347</v>
+      </c>
     </row>
-    <row r="42" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="1" t="s">
         <v>33</v>
       </c>
@@ -7717,8 +7843,11 @@
       <c r="BB42" s="10">
         <v>99</v>
       </c>
+      <c r="BC42" s="10">
+        <v>99</v>
+      </c>
     </row>
-    <row r="43" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -7881,8 +8010,11 @@
       <c r="BB43" s="10">
         <v>355</v>
       </c>
+      <c r="BC43" s="10">
+        <v>370</v>
+      </c>
     </row>
-    <row r="44" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="1" t="s">
         <v>20</v>
       </c>
@@ -8045,8 +8177,11 @@
       <c r="BB44" s="10">
         <v>296</v>
       </c>
+      <c r="BC44" s="10">
+        <v>305</v>
+      </c>
     </row>
-    <row r="45" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -8209,8 +8344,11 @@
       <c r="BB45" s="10">
         <v>24</v>
       </c>
+      <c r="BC45" s="10">
+        <v>29</v>
+      </c>
     </row>
-    <row r="46" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -8373,8 +8511,11 @@
       <c r="BB46" s="10">
         <v>226</v>
       </c>
+      <c r="BC46" s="10">
+        <v>239</v>
+      </c>
     </row>
-    <row r="47" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="1" t="s">
         <v>12</v>
       </c>
@@ -8537,8 +8678,11 @@
       <c r="BB47" s="10">
         <v>961</v>
       </c>
+      <c r="BC47" s="10">
+        <v>1006</v>
+      </c>
     </row>
-    <row r="48" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="1" t="s">
         <v>36</v>
       </c>
@@ -8701,8 +8845,11 @@
       <c r="BB48" s="10">
         <v>56</v>
       </c>
+      <c r="BC48" s="10">
+        <v>58</v>
+      </c>
     </row>
-    <row r="49" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -8865,8 +9012,11 @@
       <c r="BB49" s="10">
         <v>52</v>
       </c>
+      <c r="BC49" s="10">
+        <v>52</v>
+      </c>
     </row>
-    <row r="50" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="1" t="s">
         <v>16</v>
       </c>
@@ -9029,8 +9179,11 @@
       <c r="BB50" s="10">
         <v>713</v>
       </c>
+      <c r="BC50" s="10">
+        <v>713</v>
+      </c>
     </row>
-    <row r="51" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
@@ -9193,8 +9346,11 @@
       <c r="BB51" s="10">
         <v>870</v>
       </c>
+      <c r="BC51" s="10">
+        <v>880</v>
+      </c>
     </row>
-    <row r="52" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="1" t="s">
         <v>66</v>
       </c>
@@ -9357,8 +9513,11 @@
       <c r="BB52" s="10">
         <v>50</v>
       </c>
+      <c r="BC52" s="10">
+        <v>51</v>
+      </c>
     </row>
-    <row r="53" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="1" t="s">
         <v>18</v>
       </c>
@@ -9521,8 +9680,11 @@
       <c r="BB53" s="10">
         <v>353</v>
       </c>
+      <c r="BC53" s="10">
+        <v>362</v>
+      </c>
     </row>
-    <row r="54" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="1" t="s">
         <v>67</v>
       </c>
@@ -9685,15 +9847,18 @@
       <c r="BB54" s="11">
         <v>7</v>
       </c>
+      <c r="BC54" s="11">
+        <v>7</v>
+      </c>
     </row>
-    <row r="55" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="U55" s="7"/>
       <c r="V55" s="7"/>
       <c r="W55" s="7"/>
       <c r="AI55" s="10"/>
       <c r="AK55" s="10"/>
     </row>
-    <row r="56" spans="1:54" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:55" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="AI56" s="11"/>
       <c r="AK56" s="11"/>
     </row>

</xml_diff>